<commit_message>
Raise errors for report generator
</commit_message>
<xml_diff>
--- a/Reports/Templates/template_report.xlsx
+++ b/Reports/Templates/template_report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63d2104bdafc5139/Desktop/Programming/Python/Projects/Wilson Tool Projects/ETS/Daily Reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive\Desktop\Programming\Python\Projects\Wilson Tool Projects\ETS\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="396" documentId="8_{F9E3B5CF-DB9A-44B9-A9C6-DD2E14F1F461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDC4652F-8561-4719-A83D-4815E3EA8933}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28C4F17-781E-4554-9245-B6F568B73254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Time Taken</t>
-  </si>
-  <si>
-    <t>Fax</t>
   </si>
   <si>
     <t>Tool Type</t>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Order Status</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1045,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Workflow" displayName="Workflow" ref="A1:J200" headerRowDxfId="23" dataDxfId="21" totalsRowDxfId="20" headerRowBorderDxfId="22">
   <autoFilter ref="A1:J200" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
@@ -1058,7 +1054,7 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Designer" dataDxfId="15" totalsRowDxfId="14"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Time Taken" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Fax" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Order Status" dataDxfId="9" totalsRowDxfId="8"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tool Type" dataDxfId="7" totalsRowDxfId="6"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Repeat" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="11" xr3:uid="{A64C97EF-A5B9-42E5-972A-C4EBD704FE4D}" name="Late" dataDxfId="3" totalsRowDxfId="2"/>
@@ -1391,7 +1387,7 @@
   <dimension ref="A1:O212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A211" sqref="A211:J211"/>
+      <selection activeCell="F220" sqref="F220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -1425,19 +1421,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>8</v>
       </c>
       <c r="K1" s="8"/>
       <c r="L1" s="3"/>
@@ -3852,7 +3848,7 @@
     </row>
     <row r="201" spans="1:15" ht="16.2" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A201" s="49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B201" s="50"/>
       <c r="C201" s="50"/>
@@ -3883,14 +3879,14 @@
     </row>
     <row r="203" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A203" s="52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B203" s="53"/>
       <c r="C203" s="53"/>
       <c r="D203" s="54"/>
       <c r="E203" s="58"/>
       <c r="F203" s="55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G203" s="56"/>
       <c r="H203" s="57"/>
@@ -3902,30 +3898,30 @@
         <v>2</v>
       </c>
       <c r="B204" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C204" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C204" s="35" t="s">
-        <v>11</v>
-      </c>
       <c r="D204" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E204" s="58"/>
       <c r="F204" s="7" t="s">
         <v>2</v>
       </c>
       <c r="G204" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H204" s="19" t="s">
         <v>19</v>
-      </c>
-      <c r="H204" s="19" t="s">
-        <v>20</v>
       </c>
       <c r="I204" s="59"/>
       <c r="J204" s="60"/>
     </row>
     <row r="205" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B205" s="3">
         <f>COUNTIFS(C2:C200,"GD",I2:I200,"On Time")</f>
@@ -3941,7 +3937,7 @@
       </c>
       <c r="E205" s="58"/>
       <c r="F205" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G205" s="3">
         <f>COUNTIFS(C2:C200,"GD",G2:G200,"Form")</f>
@@ -3956,7 +3952,7 @@
     </row>
     <row r="206" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B206" s="3">
         <f>COUNTIFS(C2:C200,"ODM",I2:I200,"On Time")</f>
@@ -3972,7 +3968,7 @@
       </c>
       <c r="E206" s="58"/>
       <c r="F206" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G206" s="3">
         <f>COUNTIFS(C2:C200,"ODM",G2:G200,"Form")</f>
@@ -3987,7 +3983,7 @@
     </row>
     <row r="207" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B207" s="3">
         <f>COUNTIFS(C2:C200,"SRS",I2:I200,"On Time")</f>
@@ -4003,7 +3999,7 @@
       </c>
       <c r="E207" s="58"/>
       <c r="F207" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G207" s="3">
         <f>COUNTIFS(C2:C200,"SRS",G2:G200,"Form")</f>
@@ -4018,7 +4014,7 @@
     </row>
     <row r="208" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A208" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B208" s="3">
         <f>COUNTIFS(C2:C200,"JB",I2:I200,"On Time")</f>
@@ -4034,7 +4030,7 @@
       </c>
       <c r="E208" s="58"/>
       <c r="F208" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G208" s="3">
         <f>COUNTIFS(C2:C200,"JB",G2:G200,"Form")</f>
@@ -4049,7 +4045,7 @@
     </row>
     <row r="209" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A209" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B209" s="29">
         <f>SUM(B205:B208)</f>
@@ -4065,7 +4061,7 @@
       </c>
       <c r="E209" s="58"/>
       <c r="F209" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G209" s="29">
         <f>SUM(G205:G208)</f>

</xml_diff>